<commit_message>
Added a Gantt Chart
</commit_message>
<xml_diff>
--- a/Work_Schedule_Output.xlsx
+++ b/Work_Schedule_Output.xlsx
@@ -235,109 +235,109 @@
     <t>2025-08-04</t>
   </si>
   <si>
+    <t>2025-08-06</t>
+  </si>
+  <si>
+    <t>2025-08-08</t>
+  </si>
+  <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
+    <t>2025-08-25</t>
+  </si>
+  <si>
+    <t>2025-08-26</t>
+  </si>
+  <si>
+    <t>2025-08-27</t>
+  </si>
+  <si>
+    <t>2025-09-04</t>
+  </si>
+  <si>
+    <t>2025-09-12</t>
+  </si>
+  <si>
+    <t>2025-09-13</t>
+  </si>
+  <si>
+    <t>2025-09-15</t>
+  </si>
+  <si>
+    <t>2025-09-16</t>
+  </si>
+  <si>
+    <t>2025-08-09</t>
+  </si>
+  <si>
+    <t>2025-08-18</t>
+  </si>
+  <si>
+    <t>2025-08-28</t>
+  </si>
+  <si>
+    <t>2025-08-29</t>
+  </si>
+  <si>
+    <t>2025-09-01</t>
+  </si>
+  <si>
+    <t>2025-09-09</t>
+  </si>
+  <si>
+    <t>2025-09-17</t>
+  </si>
+  <si>
+    <t>2025-09-18</t>
+  </si>
+  <si>
+    <t>2025-09-19</t>
+  </si>
+  <si>
+    <t>2025-08-05</t>
+  </si>
+  <si>
+    <t>2025-08-13</t>
+  </si>
+  <si>
+    <t>2025-08-14</t>
+  </si>
+  <si>
+    <t>2025-08-15</t>
+  </si>
+  <si>
+    <t>2025-08-07</t>
+  </si>
+  <si>
+    <t>2025-07-29</t>
+  </si>
+  <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>2025-08-02</t>
+  </si>
+  <si>
+    <t>2025-08-23</t>
+  </si>
+  <si>
+    <t>2025-09-03</t>
+  </si>
+  <si>
+    <t>2025-09-11</t>
+  </si>
+  <si>
+    <t>2025-08-30</t>
+  </si>
+  <si>
+    <t>2025-09-08</t>
+  </si>
+  <si>
+    <t>2025-09-20</t>
+  </si>
+  <si>
     <t>2025-08-12</t>
-  </si>
-  <si>
-    <t>2025-08-14</t>
-  </si>
-  <si>
-    <t>2025-08-22</t>
-  </si>
-  <si>
-    <t>2025-08-30</t>
-  </si>
-  <si>
-    <t>2025-09-01</t>
-  </si>
-  <si>
-    <t>2025-09-02</t>
-  </si>
-  <si>
-    <t>2025-09-10</t>
-  </si>
-  <si>
-    <t>2025-09-18</t>
-  </si>
-  <si>
-    <t>2025-09-19</t>
-  </si>
-  <si>
-    <t>2025-09-20</t>
-  </si>
-  <si>
-    <t>2025-09-22</t>
-  </si>
-  <si>
-    <t>2025-08-09</t>
-  </si>
-  <si>
-    <t>2025-08-18</t>
-  </si>
-  <si>
-    <t>2025-08-26</t>
-  </si>
-  <si>
-    <t>2025-08-27</t>
-  </si>
-  <si>
-    <t>2025-08-28</t>
-  </si>
-  <si>
-    <t>2025-08-29</t>
-  </si>
-  <si>
-    <t>2025-09-09</t>
-  </si>
-  <si>
-    <t>2025-09-17</t>
-  </si>
-  <si>
-    <t>2025-08-05</t>
-  </si>
-  <si>
-    <t>2025-08-13</t>
-  </si>
-  <si>
-    <t>2025-08-15</t>
-  </si>
-  <si>
-    <t>2025-08-06</t>
-  </si>
-  <si>
-    <t>2025-08-07</t>
-  </si>
-  <si>
-    <t>2025-07-29</t>
-  </si>
-  <si>
-    <t>2025-07-31</t>
-  </si>
-  <si>
-    <t>2025-08-02</t>
-  </si>
-  <si>
-    <t>2025-08-11</t>
-  </si>
-  <si>
-    <t>2025-08-21</t>
-  </si>
-  <si>
-    <t>2025-09-23</t>
-  </si>
-  <si>
-    <t>2025-08-08</t>
-  </si>
-  <si>
-    <t>2025-08-16</t>
-  </si>
-  <si>
-    <t>2025-08-25</t>
-  </si>
-  <si>
-    <t>2025-09-08</t>
-  </si>
-  <si>
-    <t>2025-09-16</t>
   </si>
   <si>
     <t>In Progress</t>
@@ -780,7 +780,7 @@
         <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
         <v>108</v>
@@ -830,7 +830,7 @@
         <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
         <v>108</v>
@@ -880,7 +880,7 @@
         <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>108</v>
@@ -924,16 +924,16 @@
         <v>28</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H5">
         <v>48</v>
@@ -980,7 +980,7 @@
         <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
         <v>108</v>
@@ -1030,7 +1030,7 @@
         <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G7" t="s">
         <v>109</v>
@@ -1080,7 +1080,7 @@
         <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
         <v>109</v>
@@ -1230,7 +1230,7 @@
         <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="G11" t="s">
         <v>109</v>
@@ -1280,7 +1280,7 @@
         <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
         <v>109</v>
@@ -1480,7 +1480,7 @@
         <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
         <v>111</v>
@@ -1530,7 +1530,7 @@
         <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
         <v>108</v>
@@ -1580,7 +1580,7 @@
         <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s">
         <v>108</v>
@@ -1630,7 +1630,7 @@
         <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
         <v>109</v>
@@ -1680,7 +1680,7 @@
         <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G20" t="s">
         <v>109</v>
@@ -1730,7 +1730,7 @@
         <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
         <v>109</v>
@@ -1777,10 +1777,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s">
         <v>110</v>
@@ -1827,10 +1827,10 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G23" t="s">
         <v>110</v>
@@ -1877,10 +1877,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
         <v>110</v>
@@ -1927,10 +1927,10 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="G25" t="s">
         <v>111</v>
@@ -1977,10 +1977,10 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
         <v>109</v>
@@ -2027,10 +2027,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="G27" t="s">
         <v>109</v>
@@ -2077,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s">
         <v>110</v>
@@ -2127,10 +2127,10 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G29" t="s">
         <v>110</v>
@@ -2177,10 +2177,10 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F30" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="G30" t="s">
         <v>111</v>
@@ -2277,10 +2277,10 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F32" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="G32" t="s">
         <v>109</v>
@@ -2327,10 +2327,10 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
         <v>110</v>
@@ -2377,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
         <v>110</v>
@@ -2427,10 +2427,10 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G35" t="s">
         <v>111</v>
@@ -2480,7 +2480,7 @@
         <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="G36" t="s">
         <v>109</v>
@@ -2527,10 +2527,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s">
         <v>110</v>
@@ -2577,10 +2577,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F38" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
         <v>110</v>
@@ -2677,10 +2677,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G40" t="s">
         <v>110</v>
@@ -2727,10 +2727,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="G41" t="s">
         <v>110</v>
@@ -2777,10 +2777,10 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="G42" t="s">
         <v>111</v>
@@ -2830,7 +2830,7 @@
         <v>84</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G43" t="s">
         <v>109</v>
@@ -2880,7 +2880,7 @@
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="G44" t="s">
         <v>109</v>
@@ -2927,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F45" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G45" t="s">
         <v>110</v>

</xml_diff>